<commit_message>
Añadido de campos EPIGRAFE_TASA_052/062. Cambios en el excel (NO LLEVA= N/A). Actualizacion DB
</commit_message>
<xml_diff>
--- a/01-carga-excel/mysql/docs/excel-cod.xlsx
+++ b/01-carga-excel/mysql/docs/excel-cod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29607"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmunoz\trabajo\proyectos\LKS\FP\carga-excel-python\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{840D80A8-304A-41CA-A92A-7A09B7CA7B07}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44D0DD51-F815-40E4-81EC-22E36C093D3F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="10" activeTab="10" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="13" activeTab="13" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
   </bookViews>
   <sheets>
     <sheet name="EX00" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6248" uniqueCount="1277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6248" uniqueCount="1276">
   <si>
     <t>MODELO</t>
   </si>
@@ -3991,9 +3991,6 @@
     <t>2.5.2</t>
   </si>
   <si>
-    <t>NO LLEVA</t>
-  </si>
-  <si>
     <t>IABAJAKABA</t>
   </si>
   <si>
@@ -4298,7 +4295,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4506,8 +4503,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4595,6 +4598,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4800,7 +4809,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="338">
+  <cellXfs count="340">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5753,10 +5762,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="33" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6465,8 +6480,8 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="E28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="F22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -14594,8 +14609,8 @@
   </sheetPr>
   <dimension ref="A1:AS25"/>
   <sheetViews>
-    <sheetView topLeftCell="E17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="14.45"/>
@@ -14609,7 +14624,7 @@
     <col min="16" max="16384" width="10.85546875" style="182"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" customFormat="1" ht="110.45">
+    <row r="1" spans="1:45" customFormat="1" ht="108">
       <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
@@ -14746,7 +14761,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="2" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A2" s="305" t="s">
         <v>1168</v>
       </c>
@@ -14795,10 +14810,10 @@
         <v>1175</v>
       </c>
       <c r="T2" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U2" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V2" s="315" t="s">
         <v>236</v>
@@ -14826,7 +14841,7 @@
         <v>331</v>
       </c>
       <c r="AE2" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF2" s="306" t="s">
         <v>399</v>
@@ -14835,10 +14850,10 @@
         <v>209</v>
       </c>
       <c r="AH2" s="36" t="s">
+        <v>1177</v>
+      </c>
+      <c r="AI2" s="306" t="s">
         <v>1178</v>
-      </c>
-      <c r="AI2" s="306" t="s">
-        <v>1179</v>
       </c>
       <c r="AJ2" s="306" t="s">
         <v>336</v>
@@ -14857,20 +14872,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="3" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="3" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A3" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B3" s="307"/>
       <c r="C3" s="307"/>
       <c r="D3" s="308" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="E3" s="309" t="s">
         <v>1170</v>
       </c>
       <c r="F3" s="310" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="G3" s="307" t="s">
         <v>566</v>
@@ -14882,13 +14897,13 @@
         <v>29</v>
       </c>
       <c r="J3" s="311" t="s">
+        <v>1181</v>
+      </c>
+      <c r="K3" s="306" t="s">
         <v>1182</v>
       </c>
-      <c r="K3" s="306" t="s">
+      <c r="L3" s="307" t="s">
         <v>1183</v>
-      </c>
-      <c r="L3" s="307" t="s">
-        <v>1184</v>
       </c>
       <c r="M3" s="307" t="s">
         <v>201</v>
@@ -14900,16 +14915,16 @@
         <v>71364</v>
       </c>
       <c r="P3" s="307"/>
-      <c r="Q3" s="307"/>
+      <c r="Q3" s="336"/>
       <c r="R3" s="307"/>
       <c r="S3" s="331" t="s">
         <v>1175</v>
       </c>
       <c r="T3" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U3" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V3" s="315" t="s">
         <v>236</v>
@@ -14937,7 +14952,7 @@
         <v>331</v>
       </c>
       <c r="AE3" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF3" s="306" t="s">
         <v>399</v>
@@ -14949,7 +14964,7 @@
         <v>210</v>
       </c>
       <c r="AI3" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ3" s="306" t="s">
         <v>336</v>
@@ -14968,20 +14983,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="4" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A4" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B4" s="306"/>
       <c r="C4" s="307"/>
       <c r="D4" s="308" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E4" s="310" t="s">
         <v>1185</v>
       </c>
-      <c r="E4" s="310" t="s">
+      <c r="F4" s="317" t="s">
         <v>1186</v>
-      </c>
-      <c r="F4" s="317" t="s">
-        <v>1187</v>
       </c>
       <c r="G4" s="307" t="s">
         <v>566</v>
@@ -14993,13 +15008,13 @@
         <v>29</v>
       </c>
       <c r="J4" s="318" t="s">
+        <v>1187</v>
+      </c>
+      <c r="K4" s="307" t="s">
         <v>1188</v>
       </c>
-      <c r="K4" s="307" t="s">
+      <c r="L4" s="306" t="s">
         <v>1189</v>
-      </c>
-      <c r="L4" s="306" t="s">
-        <v>1190</v>
       </c>
       <c r="M4" s="307" t="s">
         <v>201</v>
@@ -15017,10 +15032,10 @@
         <v>1175</v>
       </c>
       <c r="T4" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U4" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V4" s="306" t="s">
         <v>53</v>
@@ -15048,7 +15063,7 @@
         <v>221</v>
       </c>
       <c r="AE4" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF4" s="306" t="s">
         <v>399</v>
@@ -15060,7 +15075,7 @@
         <v>210</v>
       </c>
       <c r="AI4" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ4" s="306" t="s">
         <v>336</v>
@@ -15079,20 +15094,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="5" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="5" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A5" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B5" s="307"/>
       <c r="C5" s="307"/>
       <c r="D5" s="308" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E5" s="310" t="s">
+        <v>1185</v>
+      </c>
+      <c r="F5" s="309" t="s">
         <v>1191</v>
-      </c>
-      <c r="E5" s="310" t="s">
-        <v>1186</v>
-      </c>
-      <c r="F5" s="309" t="s">
-        <v>1192</v>
       </c>
       <c r="G5" s="307" t="s">
         <v>566</v>
@@ -15104,13 +15119,13 @@
         <v>29</v>
       </c>
       <c r="J5" s="318" t="s">
+        <v>1192</v>
+      </c>
+      <c r="K5" s="319" t="s">
         <v>1193</v>
       </c>
-      <c r="K5" s="319" t="s">
+      <c r="L5" s="320" t="s">
         <v>1194</v>
-      </c>
-      <c r="L5" s="320" t="s">
-        <v>1195</v>
       </c>
       <c r="M5" s="307" t="s">
         <v>201</v>
@@ -15128,16 +15143,16 @@
         <v>1175</v>
       </c>
       <c r="T5" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U5" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V5" s="322" t="s">
         <v>236</v>
       </c>
       <c r="W5" s="321" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="X5" s="321" t="s">
         <v>53</v>
@@ -15159,7 +15174,7 @@
         <v>221</v>
       </c>
       <c r="AE5" s="321" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF5" s="323" t="s">
         <v>399</v>
@@ -15168,10 +15183,10 @@
         <v>209</v>
       </c>
       <c r="AH5" s="36" t="s">
+        <v>1177</v>
+      </c>
+      <c r="AI5" s="323" t="s">
         <v>1178</v>
-      </c>
-      <c r="AI5" s="323" t="s">
-        <v>1179</v>
       </c>
       <c r="AJ5" s="323" t="s">
         <v>336</v>
@@ -15190,20 +15205,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="6" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="6" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A6" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B6" s="307"/>
       <c r="C6" s="307"/>
       <c r="D6" s="308" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="E6" s="310" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="F6" s="310" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="G6" s="307" t="s">
         <v>566</v>
@@ -15214,14 +15229,14 @@
       <c r="I6" s="307" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="318" t="s">
-        <v>1193</v>
+      <c r="J6" s="339" t="s">
+        <v>1192</v>
       </c>
       <c r="K6" s="307" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="L6" s="307" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="M6" s="307" t="s">
         <v>201</v>
@@ -15239,16 +15254,16 @@
         <v>1175</v>
       </c>
       <c r="T6" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U6" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V6" s="322" t="s">
         <v>236</v>
       </c>
       <c r="W6" s="321" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="X6" s="321" t="s">
         <v>53</v>
@@ -15270,7 +15285,7 @@
         <v>221</v>
       </c>
       <c r="AE6" s="321" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF6" s="323" t="s">
         <v>399</v>
@@ -15282,7 +15297,7 @@
         <v>210</v>
       </c>
       <c r="AI6" s="323" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ6" s="323" t="s">
         <v>336</v>
@@ -15301,20 +15316,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="7" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="7" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A7" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B7" s="306"/>
       <c r="C7" s="307"/>
       <c r="D7" s="308" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="E7" s="310" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="F7" s="310" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="G7" s="307" t="s">
         <v>566</v>
@@ -15326,13 +15341,13 @@
         <v>29</v>
       </c>
       <c r="J7" s="318" t="s">
+        <v>1199</v>
+      </c>
+      <c r="K7" s="307" t="s">
         <v>1200</v>
       </c>
-      <c r="K7" s="307" t="s">
+      <c r="L7" s="306" t="s">
         <v>1201</v>
-      </c>
-      <c r="L7" s="306" t="s">
-        <v>1202</v>
       </c>
       <c r="M7" s="307" t="s">
         <v>201</v>
@@ -15350,10 +15365,10 @@
         <v>1175</v>
       </c>
       <c r="T7" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U7" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V7" s="306" t="s">
         <v>53</v>
@@ -15381,7 +15396,7 @@
         <v>221</v>
       </c>
       <c r="AE7" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF7" s="306" t="s">
         <v>399</v>
@@ -15393,7 +15408,7 @@
         <v>210</v>
       </c>
       <c r="AI7" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ7" s="306" t="s">
         <v>336</v>
@@ -15412,20 +15427,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:45" s="324" customFormat="1" ht="41.45">
+    <row r="8" spans="1:45" s="324" customFormat="1" ht="40.5">
       <c r="A8" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B8" s="308"/>
       <c r="C8" s="308"/>
       <c r="D8" s="308" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E8" s="317" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F8" s="317" t="s">
         <v>1203</v>
-      </c>
-      <c r="F8" s="317" t="s">
-        <v>1204</v>
       </c>
       <c r="G8" s="306" t="s">
         <v>566</v>
@@ -15437,13 +15452,13 @@
         <v>29</v>
       </c>
       <c r="J8" s="311" t="s">
+        <v>1204</v>
+      </c>
+      <c r="K8" s="306" t="s">
+        <v>1193</v>
+      </c>
+      <c r="L8" s="313" t="s">
         <v>1205</v>
-      </c>
-      <c r="K8" s="306" t="s">
-        <v>1194</v>
-      </c>
-      <c r="L8" s="313" t="s">
-        <v>1206</v>
       </c>
       <c r="M8" s="306" t="s">
         <v>201</v>
@@ -15458,13 +15473,13 @@
       <c r="Q8" s="306"/>
       <c r="R8" s="306"/>
       <c r="S8" s="331" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="T8" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U8" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V8" s="306" t="s">
         <v>236</v>
@@ -15492,7 +15507,7 @@
         <v>331</v>
       </c>
       <c r="AE8" s="306" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF8" s="306" t="s">
         <v>399</v>
@@ -15501,10 +15516,10 @@
         <v>209</v>
       </c>
       <c r="AH8" s="36" t="s">
+        <v>1177</v>
+      </c>
+      <c r="AI8" s="306" t="s">
         <v>1178</v>
-      </c>
-      <c r="AI8" s="306" t="s">
-        <v>1179</v>
       </c>
       <c r="AJ8" s="306" t="s">
         <v>336</v>
@@ -15523,20 +15538,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="9" spans="1:45" s="316" customFormat="1" ht="27">
       <c r="A9" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B9" s="308"/>
       <c r="C9" s="308"/>
       <c r="D9" s="308" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="E9" s="317" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F9" s="317" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="G9" s="306" t="s">
         <v>566</v>
@@ -15548,13 +15563,13 @@
         <v>29</v>
       </c>
       <c r="J9" s="311" t="s">
+        <v>1208</v>
+      </c>
+      <c r="K9" s="306" t="s">
+        <v>1197</v>
+      </c>
+      <c r="L9" s="313" t="s">
         <v>1209</v>
-      </c>
-      <c r="K9" s="306" t="s">
-        <v>1198</v>
-      </c>
-      <c r="L9" s="313" t="s">
-        <v>1210</v>
       </c>
       <c r="M9" s="306" t="s">
         <v>201</v>
@@ -15569,13 +15584,13 @@
       <c r="Q9" s="306"/>
       <c r="R9" s="306"/>
       <c r="S9" s="331" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="T9" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U9" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V9" s="306" t="s">
         <v>236</v>
@@ -15603,7 +15618,7 @@
         <v>221</v>
       </c>
       <c r="AE9" s="306" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF9" s="306" t="s">
         <v>399</v>
@@ -15615,7 +15630,7 @@
         <v>210</v>
       </c>
       <c r="AI9" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ9" s="306" t="s">
         <v>336</v>
@@ -15634,20 +15649,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="10" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="10" spans="1:45" s="316" customFormat="1" ht="27">
       <c r="A10" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B10" s="307"/>
       <c r="C10" s="307"/>
       <c r="D10" s="308" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="E10" s="317" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F10" s="317" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="G10" s="307" t="s">
         <v>566</v>
@@ -15659,13 +15674,13 @@
         <v>29</v>
       </c>
       <c r="J10" s="318" t="s">
+        <v>1211</v>
+      </c>
+      <c r="K10" s="307" t="s">
+        <v>1200</v>
+      </c>
+      <c r="L10" s="307" t="s">
         <v>1212</v>
-      </c>
-      <c r="K10" s="307" t="s">
-        <v>1201</v>
-      </c>
-      <c r="L10" s="307" t="s">
-        <v>1213</v>
       </c>
       <c r="M10" s="307" t="s">
         <v>201</v>
@@ -15680,13 +15695,13 @@
       <c r="Q10" s="307"/>
       <c r="R10" s="307"/>
       <c r="S10" s="331" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="T10" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U10" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V10" s="306" t="s">
         <v>53</v>
@@ -15714,7 +15729,7 @@
         <v>221</v>
       </c>
       <c r="AE10" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF10" s="306" t="s">
         <v>399</v>
@@ -15726,7 +15741,7 @@
         <v>210</v>
       </c>
       <c r="AI10" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ10" s="306" t="s">
         <v>336</v>
@@ -15745,20 +15760,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="11" spans="1:45" s="327" customFormat="1" ht="41.45">
+    <row r="11" spans="1:45" s="327" customFormat="1" ht="40.5">
       <c r="A11" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B11" s="308"/>
       <c r="C11" s="308"/>
       <c r="D11" s="308" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E11" s="310" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F11" s="309" t="s">
         <v>1214</v>
-      </c>
-      <c r="F11" s="309" t="s">
-        <v>1215</v>
       </c>
       <c r="G11" s="306" t="s">
         <v>566</v>
@@ -15771,10 +15786,10 @@
       </c>
       <c r="J11" s="325"/>
       <c r="K11" s="326" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="L11" s="326" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="M11" s="306" t="s">
         <v>201</v>
@@ -15792,10 +15807,10 @@
         <v>1175</v>
       </c>
       <c r="T11" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U11" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V11" s="306" t="s">
         <v>236</v>
@@ -15826,7 +15841,7 @@
       <c r="AF11" s="306"/>
       <c r="AG11" s="306"/>
       <c r="AH11" s="36" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AI11" s="306"/>
       <c r="AJ11" s="306"/>
@@ -15840,20 +15855,20 @@
       <c r="AR11" s="306"/>
       <c r="AS11" s="306"/>
     </row>
-    <row r="12" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="12" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A12" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B12" s="308"/>
       <c r="C12" s="308"/>
       <c r="D12" s="308" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E12" s="310" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="F12" s="317" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="G12" s="306" t="s">
         <v>566</v>
@@ -15865,13 +15880,13 @@
         <v>29</v>
       </c>
       <c r="J12" s="311" t="s">
+        <v>1217</v>
+      </c>
+      <c r="K12" s="306" t="s">
+        <v>1193</v>
+      </c>
+      <c r="L12" s="313" t="s">
         <v>1218</v>
-      </c>
-      <c r="K12" s="306" t="s">
-        <v>1194</v>
-      </c>
-      <c r="L12" s="313" t="s">
-        <v>1219</v>
       </c>
       <c r="M12" s="307" t="s">
         <v>201</v>
@@ -15889,10 +15904,10 @@
         <v>1175</v>
       </c>
       <c r="T12" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U12" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V12" s="315" t="s">
         <v>236</v>
@@ -15923,7 +15938,7 @@
       <c r="AF12" s="306"/>
       <c r="AG12" s="306"/>
       <c r="AH12" s="36" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AI12" s="306"/>
       <c r="AJ12" s="306"/>
@@ -15937,20 +15952,20 @@
       <c r="AR12" s="306"/>
       <c r="AS12" s="306"/>
     </row>
-    <row r="13" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="13" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A13" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B13" s="308"/>
       <c r="C13" s="308"/>
       <c r="D13" s="308" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="E13" s="310" t="s">
+        <v>1213</v>
+      </c>
+      <c r="F13" s="309" t="s">
         <v>1214</v>
-      </c>
-      <c r="F13" s="309" t="s">
-        <v>1215</v>
       </c>
       <c r="G13" s="306" t="s">
         <v>566</v>
@@ -15963,10 +15978,10 @@
       </c>
       <c r="J13" s="325"/>
       <c r="K13" s="326" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="L13" s="326" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="M13" s="306" t="s">
         <v>201</v>
@@ -15984,10 +15999,10 @@
         <v>1175</v>
       </c>
       <c r="T13" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U13" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V13" s="306" t="s">
         <v>236</v>
@@ -16032,20 +16047,20 @@
       <c r="AR13" s="306"/>
       <c r="AS13" s="306"/>
     </row>
-    <row r="14" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="14" spans="1:45" s="316" customFormat="1" ht="40.5">
       <c r="A14" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B14" s="308"/>
       <c r="C14" s="308"/>
       <c r="D14" s="308" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="E14" s="310" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="F14" s="317" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="G14" s="306" t="s">
         <v>566</v>
@@ -16057,13 +16072,13 @@
         <v>29</v>
       </c>
       <c r="J14" s="311" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K14" s="306" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="L14" s="313" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="M14" s="307" t="s">
         <v>201</v>
@@ -16081,10 +16096,10 @@
         <v>1175</v>
       </c>
       <c r="T14" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U14" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V14" s="315" t="s">
         <v>236</v>
@@ -16129,20 +16144,20 @@
       <c r="AR14" s="306"/>
       <c r="AS14" s="306"/>
     </row>
-    <row r="15" spans="1:45" s="285" customFormat="1" ht="27.6">
+    <row r="15" spans="1:45" s="285" customFormat="1" ht="27">
       <c r="A15" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B15" s="306"/>
       <c r="C15" s="307"/>
       <c r="D15" s="308" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E15" s="309" t="s">
         <v>1221</v>
       </c>
-      <c r="E15" s="309" t="s">
+      <c r="F15" s="310" t="s">
         <v>1222</v>
-      </c>
-      <c r="F15" s="310" t="s">
-        <v>1223</v>
       </c>
       <c r="G15" s="307" t="s">
         <v>566</v>
@@ -16155,10 +16170,10 @@
       </c>
       <c r="J15" s="328"/>
       <c r="K15" s="315" t="s">
+        <v>1223</v>
+      </c>
+      <c r="L15" s="306" t="s">
         <v>1224</v>
-      </c>
-      <c r="L15" s="306" t="s">
-        <v>1225</v>
       </c>
       <c r="M15" s="307" t="s">
         <v>201</v>
@@ -16176,10 +16191,10 @@
         <v>1175</v>
       </c>
       <c r="T15" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U15" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V15" s="307" t="s">
         <v>236</v>
@@ -16208,7 +16223,7 @@
       <c r="AF15" s="306"/>
       <c r="AG15" s="307"/>
       <c r="AH15" s="36" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AI15" s="306"/>
       <c r="AJ15" s="306"/>
@@ -16222,20 +16237,20 @@
       <c r="AR15" s="306"/>
       <c r="AS15" s="306"/>
     </row>
-    <row r="16" spans="1:45" s="285" customFormat="1" ht="41.45">
+    <row r="16" spans="1:45" s="285" customFormat="1" ht="40.5">
       <c r="A16" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B16" s="306"/>
       <c r="C16" s="307"/>
       <c r="D16" s="308" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="E16" s="309" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="F16" s="310" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="G16" s="307" t="s">
         <v>566</v>
@@ -16247,13 +16262,13 @@
         <v>29</v>
       </c>
       <c r="J16" s="318" t="s">
+        <v>1226</v>
+      </c>
+      <c r="K16" s="315" t="s">
+        <v>1223</v>
+      </c>
+      <c r="L16" s="313" t="s">
         <v>1227</v>
-      </c>
-      <c r="K16" s="315" t="s">
-        <v>1224</v>
-      </c>
-      <c r="L16" s="313" t="s">
-        <v>1228</v>
       </c>
       <c r="M16" s="307" t="s">
         <v>201</v>
@@ -16271,10 +16286,10 @@
         <v>1175</v>
       </c>
       <c r="T16" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U16" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V16" s="315" t="s">
         <v>236</v>
@@ -16302,7 +16317,7 @@
         <v>221</v>
       </c>
       <c r="AE16" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF16" s="306" t="s">
         <v>399</v>
@@ -16311,10 +16326,10 @@
         <v>209</v>
       </c>
       <c r="AH16" s="36" t="s">
+        <v>1177</v>
+      </c>
+      <c r="AI16" s="306" t="s">
         <v>1178</v>
-      </c>
-      <c r="AI16" s="306" t="s">
-        <v>1179</v>
       </c>
       <c r="AJ16" s="306" t="s">
         <v>336</v>
@@ -16333,7 +16348,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="17" spans="1:45" customFormat="1" ht="41.45">
+    <row r="17" spans="1:45" customFormat="1" ht="40.5">
       <c r="A17" s="305" t="s">
         <v>1168</v>
       </c>
@@ -16343,10 +16358,10 @@
         <v>1169</v>
       </c>
       <c r="E17" s="310" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F17" s="309" t="s">
         <v>1229</v>
-      </c>
-      <c r="F17" s="309" t="s">
-        <v>1230</v>
       </c>
       <c r="G17" s="306" t="s">
         <v>566</v>
@@ -16358,13 +16373,13 @@
         <v>29</v>
       </c>
       <c r="J17" s="311" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="K17" s="306" t="s">
         <v>1173</v>
       </c>
       <c r="L17" s="313" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="M17" s="306" t="s">
         <v>201</v>
@@ -16382,10 +16397,10 @@
         <v>1175</v>
       </c>
       <c r="T17" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U17" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V17" s="306" t="s">
         <v>236</v>
@@ -16416,7 +16431,7 @@
       <c r="AF17" s="306"/>
       <c r="AG17" s="306"/>
       <c r="AH17" s="36" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AI17" s="306"/>
       <c r="AJ17" s="306"/>
@@ -16430,7 +16445,7 @@
       <c r="AR17" s="306"/>
       <c r="AS17" s="306"/>
     </row>
-    <row r="18" spans="1:45" customFormat="1" ht="27.6">
+    <row r="18" spans="1:45" customFormat="1" ht="27">
       <c r="A18" s="305" t="s">
         <v>1168</v>
       </c>
@@ -16440,10 +16455,10 @@
         <v>1169</v>
       </c>
       <c r="E18" s="310" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="F18" s="309" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="G18" s="306" t="s">
         <v>566</v>
@@ -16459,7 +16474,7 @@
         <v>1173</v>
       </c>
       <c r="L18" s="313" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="M18" s="306" t="s">
         <v>201</v>
@@ -16477,10 +16492,10 @@
         <v>1175</v>
       </c>
       <c r="T18" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U18" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V18" s="307" t="s">
         <v>236</v>
@@ -16509,7 +16524,7 @@
       <c r="AF18" s="306"/>
       <c r="AG18" s="306"/>
       <c r="AH18" s="36" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AI18" s="306"/>
       <c r="AJ18" s="306"/>
@@ -16523,7 +16538,7 @@
       <c r="AR18" s="306"/>
       <c r="AS18" s="306"/>
     </row>
-    <row r="19" spans="1:45" customFormat="1" ht="41.45">
+    <row r="19" spans="1:45" customFormat="1" ht="40.5">
       <c r="A19" s="305" t="s">
         <v>1168</v>
       </c>
@@ -16533,10 +16548,10 @@
         <v>1169</v>
       </c>
       <c r="E19" s="310" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="F19" s="309" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="G19" s="306" t="s">
         <v>566</v>
@@ -16552,7 +16567,7 @@
         <v>1173</v>
       </c>
       <c r="L19" s="326" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="M19" s="306" t="s">
         <v>201</v>
@@ -16570,10 +16585,10 @@
         <v>1175</v>
       </c>
       <c r="T19" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U19" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V19" s="306" t="s">
         <v>236</v>
@@ -16604,7 +16619,7 @@
       <c r="AF19" s="306"/>
       <c r="AG19" s="306"/>
       <c r="AH19" s="36" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AI19" s="306"/>
       <c r="AJ19" s="306"/>
@@ -16618,7 +16633,7 @@
       <c r="AR19" s="306"/>
       <c r="AS19" s="306"/>
     </row>
-    <row r="20" spans="1:45" customFormat="1" ht="41.45">
+    <row r="20" spans="1:45" customFormat="1" ht="27">
       <c r="A20" s="305" t="s">
         <v>1168</v>
       </c>
@@ -16628,10 +16643,10 @@
         <v>1169</v>
       </c>
       <c r="E20" s="310" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="F20" s="309" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="G20" s="306" t="s">
         <v>566</v>
@@ -16647,7 +16662,7 @@
         <v>1173</v>
       </c>
       <c r="L20" s="306" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="M20" s="306" t="s">
         <v>201</v>
@@ -16665,10 +16680,10 @@
         <v>1175</v>
       </c>
       <c r="T20" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U20" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V20" s="307" t="s">
         <v>236</v>
@@ -16697,7 +16712,7 @@
       <c r="AF20" s="306"/>
       <c r="AG20" s="306"/>
       <c r="AH20" s="36" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="AI20" s="306"/>
       <c r="AJ20" s="306"/>
@@ -16711,20 +16726,20 @@
       <c r="AR20" s="306"/>
       <c r="AS20" s="306"/>
     </row>
-    <row r="21" spans="1:45" customFormat="1" ht="41.45">
+    <row r="21" spans="1:45" customFormat="1" ht="27">
       <c r="A21" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B21" s="307"/>
       <c r="C21" s="307"/>
       <c r="D21" s="308" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E21" s="309" t="s">
         <v>1238</v>
       </c>
-      <c r="E21" s="309" t="s">
+      <c r="F21" s="309" t="s">
         <v>1239</v>
-      </c>
-      <c r="F21" s="309" t="s">
-        <v>1240</v>
       </c>
       <c r="G21" s="307" t="s">
         <v>566</v>
@@ -16736,13 +16751,13 @@
         <v>29</v>
       </c>
       <c r="J21" s="311" t="s">
+        <v>1240</v>
+      </c>
+      <c r="K21" s="307" t="s">
         <v>1241</v>
       </c>
-      <c r="K21" s="307" t="s">
+      <c r="L21" s="313" t="s">
         <v>1242</v>
-      </c>
-      <c r="L21" s="313" t="s">
-        <v>1243</v>
       </c>
       <c r="M21" s="307" t="s">
         <v>201</v>
@@ -16757,13 +16772,13 @@
       <c r="Q21" s="307"/>
       <c r="R21" s="307"/>
       <c r="S21" s="331" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="T21" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U21" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V21" s="315" t="s">
         <v>236</v>
@@ -16791,7 +16806,7 @@
         <v>221</v>
       </c>
       <c r="AE21" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF21" s="306" t="s">
         <v>399</v>
@@ -16803,7 +16818,7 @@
         <v>210</v>
       </c>
       <c r="AI21" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ21" s="306" t="s">
         <v>336</v>
@@ -16822,20 +16837,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="22" spans="1:45" customFormat="1" ht="41.45">
+    <row r="22" spans="1:45" customFormat="1" ht="27">
       <c r="A22" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B22" s="306"/>
       <c r="C22" s="307"/>
       <c r="D22" s="308" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E22" s="310" t="s">
         <v>1245</v>
       </c>
-      <c r="E22" s="310" t="s">
+      <c r="F22" s="317" t="s">
         <v>1246</v>
-      </c>
-      <c r="F22" s="317" t="s">
-        <v>1247</v>
       </c>
       <c r="G22" s="307" t="s">
         <v>566</v>
@@ -16847,13 +16862,13 @@
         <v>131</v>
       </c>
       <c r="J22" s="311" t="s">
+        <v>1247</v>
+      </c>
+      <c r="K22" s="306" t="s">
+        <v>1231</v>
+      </c>
+      <c r="L22" s="306" t="s">
         <v>1248</v>
-      </c>
-      <c r="K22" s="306" t="s">
-        <v>1232</v>
-      </c>
-      <c r="L22" s="306" t="s">
-        <v>1249</v>
       </c>
       <c r="M22" s="307" t="s">
         <v>201</v>
@@ -16868,13 +16883,13 @@
       <c r="Q22" s="307"/>
       <c r="R22" s="306"/>
       <c r="S22" s="331" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="T22" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U22" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V22" s="315" t="s">
         <v>236</v>
@@ -16902,7 +16917,7 @@
         <v>221</v>
       </c>
       <c r="AE22" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF22" s="306" t="s">
         <v>399</v>
@@ -16914,7 +16929,7 @@
         <v>210</v>
       </c>
       <c r="AI22" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ22" s="306" t="s">
         <v>336</v>
@@ -16933,20 +16948,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="23" spans="1:45" customFormat="1" ht="41.45">
+    <row r="23" spans="1:45" customFormat="1" ht="27">
       <c r="A23" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B23" s="306"/>
       <c r="C23" s="307"/>
       <c r="D23" s="308" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="E23" s="310" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F23" s="317" t="s">
         <v>1250</v>
-      </c>
-      <c r="F23" s="317" t="s">
-        <v>1251</v>
       </c>
       <c r="G23" s="307" t="s">
         <v>566</v>
@@ -16959,10 +16974,10 @@
       </c>
       <c r="J23" s="325"/>
       <c r="K23" s="312" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="L23" s="329" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="M23" s="307" t="s">
         <v>201</v>
@@ -16977,13 +16992,13 @@
       <c r="Q23" s="307"/>
       <c r="R23" s="306"/>
       <c r="S23" s="331" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="T23" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U23" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V23" s="315" t="s">
         <v>236</v>
@@ -17011,7 +17026,7 @@
         <v>221</v>
       </c>
       <c r="AE23" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF23" s="306" t="s">
         <v>399</v>
@@ -17023,7 +17038,7 @@
         <v>210</v>
       </c>
       <c r="AI23" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ23" s="306" t="s">
         <v>336</v>
@@ -17042,38 +17057,38 @@
         <v>399</v>
       </c>
     </row>
-    <row r="24" spans="1:45" s="316" customFormat="1" ht="41.45">
+    <row r="24" spans="1:45" s="316" customFormat="1" ht="27">
       <c r="A24" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B24" s="306"/>
       <c r="C24" s="307"/>
       <c r="D24" s="308" t="s">
+        <v>1252</v>
+      </c>
+      <c r="E24" s="310" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F24" s="310" t="s">
         <v>1253</v>
-      </c>
-      <c r="E24" s="310" t="s">
-        <v>1203</v>
-      </c>
-      <c r="F24" s="310" t="s">
-        <v>1254</v>
       </c>
       <c r="G24" s="307" t="s">
         <v>566</v>
       </c>
       <c r="H24" s="306" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="I24" s="306" t="s">
         <v>131</v>
       </c>
       <c r="J24" s="318" t="s">
+        <v>1255</v>
+      </c>
+      <c r="K24" s="307" t="s">
         <v>1256</v>
       </c>
-      <c r="K24" s="307" t="s">
+      <c r="L24" s="306" t="s">
         <v>1257</v>
-      </c>
-      <c r="L24" s="306" t="s">
-        <v>1258</v>
       </c>
       <c r="M24" s="307" t="s">
         <v>201</v>
@@ -17088,13 +17103,13 @@
       <c r="Q24" s="307"/>
       <c r="R24" s="306"/>
       <c r="S24" s="332" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="T24" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U24" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V24" s="306" t="s">
         <v>53</v>
@@ -17124,7 +17139,7 @@
         <v>221</v>
       </c>
       <c r="AE24" s="307" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="AF24" s="306" t="s">
         <v>399</v>
@@ -17136,7 +17151,7 @@
         <v>210</v>
       </c>
       <c r="AI24" s="306" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="AJ24" s="306" t="s">
         <v>336</v>
@@ -17155,20 +17170,20 @@
         <v>399</v>
       </c>
     </row>
-    <row r="25" spans="1:45" s="316" customFormat="1" ht="27.6">
+    <row r="25" spans="1:45" s="316" customFormat="1" ht="27">
       <c r="A25" s="305" t="s">
         <v>1168</v>
       </c>
       <c r="B25" s="308"/>
       <c r="C25" s="308"/>
       <c r="D25" s="308" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E25" s="317" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F25" s="317" t="s">
         <v>1260</v>
-      </c>
-      <c r="E25" s="317" t="s">
-        <v>1203</v>
-      </c>
-      <c r="F25" s="317" t="s">
-        <v>1261</v>
       </c>
       <c r="G25" s="306" t="s">
         <v>566</v>
@@ -17180,13 +17195,13 @@
         <v>29</v>
       </c>
       <c r="J25" s="311" t="s">
+        <v>1261</v>
+      </c>
+      <c r="K25" s="306" t="s">
         <v>1262</v>
       </c>
-      <c r="K25" s="306" t="s">
+      <c r="L25" s="306" t="s">
         <v>1263</v>
-      </c>
-      <c r="L25" s="306" t="s">
-        <v>1264</v>
       </c>
       <c r="M25" s="306" t="s">
         <v>201</v>
@@ -17204,16 +17219,16 @@
         <v>233</v>
       </c>
       <c r="T25" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="U25" s="331" t="s">
-        <v>1176</v>
+        <v>38</v>
       </c>
       <c r="V25" s="306" t="s">
         <v>236</v>
       </c>
       <c r="W25" s="306" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="X25" s="306" t="s">
         <v>53</v>
@@ -17496,15 +17511,15 @@
     </row>
     <row r="2" spans="1:89" s="33" customFormat="1" ht="110.45">
       <c r="A2" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B2" s="178"/>
       <c r="C2" s="1"/>
       <c r="D2" s="173" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E2" s="301" t="s">
         <v>1267</v>
-      </c>
-      <c r="E2" s="301" t="s">
-        <v>1268</v>
       </c>
       <c r="F2" s="303" t="s">
         <v>641</v>
@@ -17520,13 +17535,13 @@
       </c>
       <c r="J2" s="36"/>
       <c r="K2" s="36" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="L2" s="36" t="s">
         <v>699</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="N2" s="84">
         <v>45798</v>
@@ -17587,15 +17602,15 @@
     </row>
     <row r="3" spans="1:89" s="33" customFormat="1" ht="110.45">
       <c r="A3" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B3" s="178"/>
       <c r="C3" s="1"/>
       <c r="D3" s="173" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="E3" s="301" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="F3" s="303" t="s">
         <v>641</v>
@@ -17611,13 +17626,13 @@
       </c>
       <c r="J3" s="36"/>
       <c r="K3" s="36" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="L3" s="36" t="s">
         <v>706</v>
       </c>
       <c r="M3" s="36" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="N3" s="84">
         <v>45800</v>
@@ -17678,15 +17693,15 @@
     </row>
     <row r="4" spans="1:89" s="33" customFormat="1" ht="110.45">
       <c r="A4" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B4" s="178"/>
       <c r="C4" s="1"/>
       <c r="D4" s="173" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="E4" s="301" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="F4" s="303" t="s">
         <v>641</v>
@@ -17702,13 +17717,13 @@
       </c>
       <c r="J4" s="36"/>
       <c r="K4" s="36" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="L4" s="36" t="s">
         <v>712</v>
       </c>
       <c r="M4" s="36" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="N4" s="84">
         <v>45802</v>
@@ -17769,15 +17784,15 @@
     </row>
     <row r="5" spans="1:89" s="33" customFormat="1" ht="110.45">
       <c r="A5" s="1" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="B5" s="178"/>
       <c r="C5" s="1"/>
       <c r="D5" s="173" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="E5" s="304" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F5" s="303" t="s">
         <v>641</v>
@@ -17793,13 +17808,13 @@
       </c>
       <c r="J5" s="36"/>
       <c r="K5" s="36" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="L5" s="145" t="s">
         <v>718</v>
       </c>
       <c r="M5" s="36" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="N5" s="84">
         <v>45804</v>
@@ -18384,7 +18399,7 @@
   </sheetPr>
   <dimension ref="A1:CK15"/>
   <sheetViews>
-    <sheetView topLeftCell="G13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -24671,7 +24686,7 @@
   </sheetPr>
   <dimension ref="A1:CK9"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
@@ -28417,10 +28432,10 @@
       <c r="P3" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q3" s="336" t="s">
+      <c r="Q3" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R3" s="337"/>
+      <c r="R3" s="338"/>
       <c r="S3" s="224" t="s">
         <v>694</v>
       </c>
@@ -28689,10 +28704,10 @@
       <c r="P5" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q5" s="336" t="s">
+      <c r="Q5" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R5" s="337"/>
+      <c r="R5" s="338"/>
       <c r="S5" s="147" t="s">
         <v>694</v>
       </c>
@@ -28983,10 +28998,10 @@
       <c r="P7" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q7" s="336" t="s">
+      <c r="Q7" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R7" s="337"/>
+      <c r="R7" s="338"/>
       <c r="S7" s="147" t="s">
         <v>694</v>
       </c>
@@ -29253,10 +29268,10 @@
       <c r="P9" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q9" s="336" t="s">
+      <c r="Q9" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R9" s="337"/>
+      <c r="R9" s="338"/>
       <c r="S9" s="147" t="s">
         <v>694</v>
       </c>
@@ -29523,10 +29538,10 @@
       <c r="P11" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q11" s="336" t="s">
+      <c r="Q11" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R11" s="337"/>
+      <c r="R11" s="338"/>
       <c r="S11" s="147" t="s">
         <v>694</v>
       </c>
@@ -29668,10 +29683,10 @@
       <c r="P12" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q12" s="336" t="s">
+      <c r="Q12" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R12" s="337"/>
+      <c r="R12" s="338"/>
       <c r="S12" s="147" t="s">
         <v>701</v>
       </c>
@@ -29960,10 +29975,10 @@
       <c r="P14" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q14" s="336" t="s">
+      <c r="Q14" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R14" s="337"/>
+      <c r="R14" s="338"/>
       <c r="S14" s="224" t="s">
         <v>694</v>
       </c>
@@ -30232,10 +30247,10 @@
       <c r="P16" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q16" s="336" t="s">
+      <c r="Q16" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R16" s="337"/>
+      <c r="R16" s="338"/>
       <c r="S16" s="224" t="s">
         <v>694</v>
       </c>
@@ -30502,10 +30517,10 @@
       <c r="P18" s="224" t="s">
         <v>749</v>
       </c>
-      <c r="Q18" s="336" t="s">
+      <c r="Q18" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R18" s="337"/>
+      <c r="R18" s="338"/>
       <c r="S18" s="224" t="s">
         <v>38</v>
       </c>
@@ -30649,10 +30664,10 @@
       <c r="P19" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q19" s="336" t="s">
+      <c r="Q19" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R19" s="337"/>
+      <c r="R19" s="338"/>
       <c r="S19" s="224" t="s">
         <v>751</v>
       </c>
@@ -30796,10 +30811,10 @@
       <c r="P20" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q20" s="336" t="s">
+      <c r="Q20" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R20" s="337"/>
+      <c r="R20" s="338"/>
       <c r="S20" s="224" t="s">
         <v>751</v>
       </c>
@@ -30943,10 +30958,10 @@
       <c r="P21" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q21" s="336" t="s">
+      <c r="Q21" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R21" s="337"/>
+      <c r="R21" s="338"/>
       <c r="S21" s="224" t="s">
         <v>751</v>
       </c>
@@ -31066,10 +31081,10 @@
       <c r="P22" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q22" s="336" t="s">
+      <c r="Q22" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R22" s="337"/>
+      <c r="R22" s="338"/>
       <c r="S22" s="224" t="s">
         <v>751</v>
       </c>
@@ -31189,10 +31204,10 @@
       <c r="P23" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q23" s="336" t="s">
+      <c r="Q23" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R23" s="337"/>
+      <c r="R23" s="338"/>
       <c r="S23" s="224" t="s">
         <v>751</v>
       </c>
@@ -31336,10 +31351,10 @@
       <c r="P24" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q24" s="336" t="s">
+      <c r="Q24" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R24" s="337"/>
+      <c r="R24" s="338"/>
       <c r="S24" s="224" t="s">
         <v>751</v>
       </c>
@@ -31483,10 +31498,10 @@
       <c r="P25" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q25" s="336" t="s">
+      <c r="Q25" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R25" s="337"/>
+      <c r="R25" s="338"/>
       <c r="S25" s="224" t="s">
         <v>751</v>
       </c>
@@ -31630,10 +31645,10 @@
       <c r="P26" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q26" s="336" t="s">
+      <c r="Q26" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R26" s="337"/>
+      <c r="R26" s="338"/>
       <c r="S26" s="224" t="s">
         <v>751</v>
       </c>
@@ -31777,10 +31792,10 @@
       <c r="P27" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q27" s="336" t="s">
+      <c r="Q27" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R27" s="337"/>
+      <c r="R27" s="338"/>
       <c r="S27" s="224" t="s">
         <v>751</v>
       </c>
@@ -31924,10 +31939,10 @@
       <c r="P28" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q28" s="336" t="s">
+      <c r="Q28" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R28" s="337"/>
+      <c r="R28" s="338"/>
       <c r="S28" s="224" t="s">
         <v>751</v>
       </c>
@@ -32071,10 +32086,10 @@
       <c r="P29" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q29" s="336" t="s">
+      <c r="Q29" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R29" s="337"/>
+      <c r="R29" s="338"/>
       <c r="S29" s="224" t="s">
         <v>751</v>
       </c>
@@ -32218,10 +32233,10 @@
       <c r="P30" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q30" s="336" t="s">
+      <c r="Q30" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R30" s="337"/>
+      <c r="R30" s="338"/>
       <c r="S30" s="224" t="s">
         <v>751</v>
       </c>
@@ -32365,10 +32380,10 @@
       <c r="P31" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q31" s="336" t="s">
+      <c r="Q31" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R31" s="337"/>
+      <c r="R31" s="338"/>
       <c r="S31" s="224" t="s">
         <v>38</v>
       </c>
@@ -32512,10 +32527,10 @@
       <c r="P32" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q32" s="336" t="s">
+      <c r="Q32" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R32" s="337"/>
+      <c r="R32" s="338"/>
       <c r="S32" s="224" t="s">
         <v>751</v>
       </c>
@@ -32659,10 +32674,10 @@
       <c r="P33" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q33" s="336" t="s">
+      <c r="Q33" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R33" s="337"/>
+      <c r="R33" s="338"/>
       <c r="S33" s="224" t="s">
         <v>751</v>
       </c>
@@ -32782,10 +32797,10 @@
       <c r="P34" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q34" s="336" t="s">
+      <c r="Q34" s="337" t="s">
         <v>728</v>
       </c>
-      <c r="R34" s="337"/>
+      <c r="R34" s="338"/>
       <c r="S34" s="224" t="s">
         <v>38</v>
       </c>
@@ -33054,10 +33069,10 @@
       <c r="P36" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q36" s="336" t="s">
+      <c r="Q36" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R36" s="337"/>
+      <c r="R36" s="338"/>
       <c r="S36" s="224" t="s">
         <v>694</v>
       </c>
@@ -33350,10 +33365,10 @@
       <c r="P38" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q38" s="336" t="s">
+      <c r="Q38" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R38" s="337"/>
+      <c r="R38" s="338"/>
       <c r="S38" s="224" t="s">
         <v>694</v>
       </c>
@@ -33646,10 +33661,10 @@
       <c r="P40" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q40" s="336" t="s">
+      <c r="Q40" s="337" t="s">
         <v>693</v>
       </c>
-      <c r="R40" s="337"/>
+      <c r="R40" s="338"/>
       <c r="S40" s="224" t="s">
         <v>694</v>
       </c>

</xml_diff>

<commit_message>
Añadir campo DURACION. Creacion de procedimientos almacenados(comprobaciones)
</commit_message>
<xml_diff>
--- a/01-carga-excel/mysql/docs/excel-cod.xlsx
+++ b/01-carga-excel/mysql/docs/excel-cod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmunoz\trabajo\proyectos\LKS\FP\carga-excel-python\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44D0DD51-F815-40E4-81EC-22E36C093D3F}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D40365A5-880B-4BC0-A380-754125073529}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="13" activeTab="13" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="13" activeTab="2" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
   </bookViews>
   <sheets>
     <sheet name="EX00" sheetId="1" r:id="rId1"/>
@@ -5765,13 +5765,13 @@
     <xf numFmtId="49" fontId="33" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="16" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="16" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6480,8 +6480,8 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="F22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView topLeftCell="D8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8557,7 +8557,7 @@
   </sheetPr>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -14609,7 +14609,7 @@
   </sheetPr>
   <dimension ref="A1:AS25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -15229,7 +15229,7 @@
       <c r="I6" s="307" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="339" t="s">
+      <c r="J6" s="337" t="s">
         <v>1192</v>
       </c>
       <c r="K6" s="307" t="s">
@@ -17322,7 +17322,7 @@
   </sheetPr>
   <dimension ref="A1:CK5"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -17890,7 +17890,7 @@
   </sheetPr>
   <dimension ref="A1:AS5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -18399,8 +18399,8 @@
   </sheetPr>
   <dimension ref="A1:CK15"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -20637,7 +20637,7 @@
   </sheetPr>
   <dimension ref="A1:CK30"/>
   <sheetViews>
-    <sheetView topLeftCell="B27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="S16" sqref="S16:T16"/>
     </sheetView>
   </sheetViews>
@@ -24686,7 +24686,7 @@
   </sheetPr>
   <dimension ref="A1:CK9"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
@@ -25888,7 +25888,7 @@
   </sheetPr>
   <dimension ref="A1:CI7"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -26582,7 +26582,7 @@
   </sheetPr>
   <dimension ref="A1:AS11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -28032,7 +28032,7 @@
   </sheetPr>
   <dimension ref="A1:CK44"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="H33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -28432,10 +28432,10 @@
       <c r="P3" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q3" s="337" t="s">
+      <c r="Q3" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R3" s="338"/>
+      <c r="R3" s="339"/>
       <c r="S3" s="224" t="s">
         <v>694</v>
       </c>
@@ -28704,10 +28704,10 @@
       <c r="P5" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q5" s="337" t="s">
+      <c r="Q5" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R5" s="338"/>
+      <c r="R5" s="339"/>
       <c r="S5" s="147" t="s">
         <v>694</v>
       </c>
@@ -28998,10 +28998,10 @@
       <c r="P7" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q7" s="337" t="s">
+      <c r="Q7" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R7" s="338"/>
+      <c r="R7" s="339"/>
       <c r="S7" s="147" t="s">
         <v>694</v>
       </c>
@@ -29268,10 +29268,10 @@
       <c r="P9" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q9" s="337" t="s">
+      <c r="Q9" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R9" s="338"/>
+      <c r="R9" s="339"/>
       <c r="S9" s="147" t="s">
         <v>694</v>
       </c>
@@ -29538,10 +29538,10 @@
       <c r="P11" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q11" s="337" t="s">
+      <c r="Q11" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R11" s="338"/>
+      <c r="R11" s="339"/>
       <c r="S11" s="147" t="s">
         <v>694</v>
       </c>
@@ -29683,10 +29683,10 @@
       <c r="P12" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q12" s="337" t="s">
+      <c r="Q12" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R12" s="338"/>
+      <c r="R12" s="339"/>
       <c r="S12" s="147" t="s">
         <v>701</v>
       </c>
@@ -29975,10 +29975,10 @@
       <c r="P14" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q14" s="337" t="s">
+      <c r="Q14" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R14" s="338"/>
+      <c r="R14" s="339"/>
       <c r="S14" s="224" t="s">
         <v>694</v>
       </c>
@@ -30247,10 +30247,10 @@
       <c r="P16" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q16" s="337" t="s">
+      <c r="Q16" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R16" s="338"/>
+      <c r="R16" s="339"/>
       <c r="S16" s="224" t="s">
         <v>694</v>
       </c>
@@ -30517,10 +30517,10 @@
       <c r="P18" s="224" t="s">
         <v>749</v>
       </c>
-      <c r="Q18" s="337" t="s">
+      <c r="Q18" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R18" s="338"/>
+      <c r="R18" s="339"/>
       <c r="S18" s="224" t="s">
         <v>38</v>
       </c>
@@ -30664,10 +30664,10 @@
       <c r="P19" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q19" s="337" t="s">
+      <c r="Q19" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R19" s="338"/>
+      <c r="R19" s="339"/>
       <c r="S19" s="224" t="s">
         <v>751</v>
       </c>
@@ -30811,10 +30811,10 @@
       <c r="P20" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q20" s="337" t="s">
+      <c r="Q20" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R20" s="338"/>
+      <c r="R20" s="339"/>
       <c r="S20" s="224" t="s">
         <v>751</v>
       </c>
@@ -30958,10 +30958,10 @@
       <c r="P21" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q21" s="337" t="s">
+      <c r="Q21" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R21" s="338"/>
+      <c r="R21" s="339"/>
       <c r="S21" s="224" t="s">
         <v>751</v>
       </c>
@@ -31081,10 +31081,10 @@
       <c r="P22" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q22" s="337" t="s">
+      <c r="Q22" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R22" s="338"/>
+      <c r="R22" s="339"/>
       <c r="S22" s="224" t="s">
         <v>751</v>
       </c>
@@ -31204,10 +31204,10 @@
       <c r="P23" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q23" s="337" t="s">
+      <c r="Q23" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R23" s="338"/>
+      <c r="R23" s="339"/>
       <c r="S23" s="224" t="s">
         <v>751</v>
       </c>
@@ -31351,10 +31351,10 @@
       <c r="P24" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q24" s="337" t="s">
+      <c r="Q24" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R24" s="338"/>
+      <c r="R24" s="339"/>
       <c r="S24" s="224" t="s">
         <v>751</v>
       </c>
@@ -31498,10 +31498,10 @@
       <c r="P25" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q25" s="337" t="s">
+      <c r="Q25" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R25" s="338"/>
+      <c r="R25" s="339"/>
       <c r="S25" s="224" t="s">
         <v>751</v>
       </c>
@@ -31645,10 +31645,10 @@
       <c r="P26" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q26" s="337" t="s">
+      <c r="Q26" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R26" s="338"/>
+      <c r="R26" s="339"/>
       <c r="S26" s="224" t="s">
         <v>751</v>
       </c>
@@ -31792,10 +31792,10 @@
       <c r="P27" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q27" s="337" t="s">
+      <c r="Q27" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R27" s="338"/>
+      <c r="R27" s="339"/>
       <c r="S27" s="224" t="s">
         <v>751</v>
       </c>
@@ -31939,10 +31939,10 @@
       <c r="P28" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q28" s="337" t="s">
+      <c r="Q28" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R28" s="338"/>
+      <c r="R28" s="339"/>
       <c r="S28" s="224" t="s">
         <v>751</v>
       </c>
@@ -32086,10 +32086,10 @@
       <c r="P29" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q29" s="337" t="s">
+      <c r="Q29" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R29" s="338"/>
+      <c r="R29" s="339"/>
       <c r="S29" s="224" t="s">
         <v>751</v>
       </c>
@@ -32233,10 +32233,10 @@
       <c r="P30" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q30" s="337" t="s">
+      <c r="Q30" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R30" s="338"/>
+      <c r="R30" s="339"/>
       <c r="S30" s="224" t="s">
         <v>751</v>
       </c>
@@ -32380,10 +32380,10 @@
       <c r="P31" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q31" s="337" t="s">
+      <c r="Q31" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R31" s="338"/>
+      <c r="R31" s="339"/>
       <c r="S31" s="224" t="s">
         <v>38</v>
       </c>
@@ -32527,10 +32527,10 @@
       <c r="P32" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q32" s="337" t="s">
+      <c r="Q32" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R32" s="338"/>
+      <c r="R32" s="339"/>
       <c r="S32" s="224" t="s">
         <v>751</v>
       </c>
@@ -32674,10 +32674,10 @@
       <c r="P33" s="224" t="s">
         <v>727</v>
       </c>
-      <c r="Q33" s="337" t="s">
+      <c r="Q33" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R33" s="338"/>
+      <c r="R33" s="339"/>
       <c r="S33" s="224" t="s">
         <v>751</v>
       </c>
@@ -32797,10 +32797,10 @@
       <c r="P34" s="224" t="s">
         <v>205</v>
       </c>
-      <c r="Q34" s="337" t="s">
+      <c r="Q34" s="338" t="s">
         <v>728</v>
       </c>
-      <c r="R34" s="338"/>
+      <c r="R34" s="339"/>
       <c r="S34" s="224" t="s">
         <v>38</v>
       </c>
@@ -33069,10 +33069,10 @@
       <c r="P36" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q36" s="337" t="s">
+      <c r="Q36" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R36" s="338"/>
+      <c r="R36" s="339"/>
       <c r="S36" s="224" t="s">
         <v>694</v>
       </c>
@@ -33365,10 +33365,10 @@
       <c r="P38" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q38" s="337" t="s">
+      <c r="Q38" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R38" s="338"/>
+      <c r="R38" s="339"/>
       <c r="S38" s="224" t="s">
         <v>694</v>
       </c>
@@ -33661,10 +33661,10 @@
       <c r="P40" s="224" t="s">
         <v>692</v>
       </c>
-      <c r="Q40" s="337" t="s">
+      <c r="Q40" s="338" t="s">
         <v>693</v>
       </c>
-      <c r="R40" s="338"/>
+      <c r="R40" s="339"/>
       <c r="S40" s="224" t="s">
         <v>694</v>
       </c>
@@ -34268,12 +34268,16 @@
   </sheetData>
   <autoFilter ref="A1:CK1" xr:uid="{81481555-CC8D-496A-8B62-D9F1569CF07D}"/>
   <mergeCells count="28">
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="Q16:R16"/>
@@ -34286,16 +34290,12 @@
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="Q25:R25"/>
     <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q11:R11"/>
   </mergeCells>
   <conditionalFormatting sqref="P1:R1">
     <cfRule type="expression" dxfId="28" priority="1" stopIfTrue="1">

</xml_diff>

<commit_message>
Actualizacion del campo DURACION, revalidadas los patrones indefinidos
</commit_message>
<xml_diff>
--- a/01-carga-excel/mysql/docs/excel-cod.xlsx
+++ b/01-carga-excel/mysql/docs/excel-cod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmunoz\trabajo\proyectos\LKS\FP\carga-excel-python\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D40365A5-880B-4BC0-A380-754125073529}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3949206E-1C4F-44D5-BE7C-45E2F452C269}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="13" activeTab="2" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="2" activeTab="3" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
   </bookViews>
   <sheets>
     <sheet name="EX00" sheetId="1" r:id="rId1"/>
@@ -6480,8 +6480,8 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="D8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView topLeftCell="D6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -8557,7 +8557,7 @@
   </sheetPr>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView topLeftCell="E13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -11172,7 +11172,7 @@
   </sheetPr>
   <dimension ref="A1:CK7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -11957,7 +11957,7 @@
   <dimension ref="A1:AS26"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="J8" sqref="J8:W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -14609,7 +14609,7 @@
   </sheetPr>
   <dimension ref="A1:AS25"/>
   <sheetViews>
-    <sheetView topLeftCell="G12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -17891,7 +17891,7 @@
   <dimension ref="A1:AS5"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -18399,8 +18399,8 @@
   </sheetPr>
   <dimension ref="A1:CK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -20637,8 +20637,8 @@
   </sheetPr>
   <dimension ref="A1:CK30"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16:T16"/>
+    <sheetView tabSelected="1" topLeftCell="H16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.15"/>
@@ -28032,7 +28032,7 @@
   </sheetPr>
   <dimension ref="A1:CK44"/>
   <sheetViews>
-    <sheetView topLeftCell="H33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="H26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -34268,16 +34268,12 @@
   </sheetData>
   <autoFilter ref="A1:CK1" xr:uid="{81481555-CC8D-496A-8B62-D9F1569CF07D}"/>
   <mergeCells count="28">
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q11:R11"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="Q16:R16"/>
@@ -34290,12 +34286,16 @@
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="Q25:R25"/>
     <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
   </mergeCells>
   <conditionalFormatting sqref="P1:R1">
     <cfRule type="expression" dxfId="28" priority="1" stopIfTrue="1">

</xml_diff>

<commit_message>
Añadido de Paginas Carga por Archivo y Carga por Interfaz. [CargaInterfaz] Añadido parte CRUD de creacion y consulta, faltando asi Borrado y edicion. [CargaArchivo] de momento solo implementado por excel metido "a fuego", mas adelante implementacion de pagina de subida de archivo
</commit_message>
<xml_diff>
--- a/01-carga-excel/mysql/docs/excel-cod.xlsx
+++ b/01-carga-excel/mysql/docs/excel-cod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmunoz\trabajo\proyectos\LKS\FP\carga-excel-python\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3949206E-1C4F-44D5-BE7C-45E2F452C269}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BBAC4E-EF19-4721-8525-5A55AA081AE1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="2" activeTab="3" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="3" activeTab="5" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
   </bookViews>
   <sheets>
     <sheet name="EX00" sheetId="1" r:id="rId1"/>
@@ -6480,7 +6480,7 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="D6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -8557,7 +8557,7 @@
   </sheetPr>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -10762,7 +10762,7 @@
   </sheetPr>
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -11956,8 +11956,8 @@
   </sheetPr>
   <dimension ref="A1:AS26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:W9"/>
+    <sheetView topLeftCell="D15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -18399,7 +18399,7 @@
   </sheetPr>
   <dimension ref="A1:CK15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -20637,7 +20637,7 @@
   </sheetPr>
   <dimension ref="A1:CK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -24686,7 +24686,7 @@
   </sheetPr>
   <dimension ref="A1:CK9"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
@@ -25888,8 +25888,8 @@
   </sheetPr>
   <dimension ref="A1:CI7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -25901,7 +25901,7 @@
     <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="77" customFormat="1" ht="55.15">
+    <row r="1" spans="1:87" s="77" customFormat="1" ht="53.25">
       <c r="A1" s="64" t="s">
         <v>529</v>
       </c>
@@ -25936,7 +25936,7 @@
         <v>532</v>
       </c>
       <c r="L1" s="69" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="M1" s="27" t="s">
         <v>533</v>
@@ -26582,7 +26582,7 @@
   </sheetPr>
   <dimension ref="A1:AS11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -27381,7 +27381,7 @@
   </sheetPr>
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="S2" sqref="S2:S7"/>
     </sheetView>
   </sheetViews>
@@ -28032,7 +28032,7 @@
   </sheetPr>
   <dimension ref="A1:CK44"/>
   <sheetViews>
-    <sheetView topLeftCell="H26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -34268,12 +34268,16 @@
   </sheetData>
   <autoFilter ref="A1:CK1" xr:uid="{81481555-CC8D-496A-8B62-D9F1569CF07D}"/>
   <mergeCells count="28">
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="Q16:R16"/>
@@ -34286,16 +34290,12 @@
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="Q25:R25"/>
     <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q11:R11"/>
   </mergeCells>
   <conditionalFormatting sqref="P1:R1">
     <cfRule type="expression" dxfId="28" priority="1" stopIfTrue="1">

</xml_diff>

<commit_message>
Revert "Añadido de Paginas Carga por Archivo y Carga por Interfaz. [CargaInterfaz] Añadido parte CRUD de creacion y consulta, faltando asi Borrado y edicion. [CargaArchivo] de momento solo implementado por excel metido "a fuego", mas adelante implementacion de pagina de subida de archivo"
This reverts commit 02437e9e988c6c2d38f6800da4888c6de5fcfea5.
</commit_message>
<xml_diff>
--- a/01-carga-excel/mysql/docs/excel-cod.xlsx
+++ b/01-carga-excel/mysql/docs/excel-cod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmunoz\trabajo\proyectos\LKS\FP\carga-excel-python\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BBAC4E-EF19-4721-8525-5A55AA081AE1}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{FD160B07-0254-45C5-837A-198D083F8BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3949206E-1C4F-44D5-BE7C-45E2F452C269}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="3" activeTab="5" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="2" activeTab="3" xr2:uid="{985A6DF8-F51D-4D3E-B1AA-DA801117F226}"/>
   </bookViews>
   <sheets>
     <sheet name="EX00" sheetId="1" r:id="rId1"/>
@@ -6480,7 +6480,7 @@
   </sheetPr>
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -8557,7 +8557,7 @@
   </sheetPr>
   <dimension ref="A1:AS20"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
@@ -10762,7 +10762,7 @@
   </sheetPr>
   <dimension ref="A1:AI12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -11956,8 +11956,8 @@
   </sheetPr>
   <dimension ref="A1:AS26"/>
   <sheetViews>
-    <sheetView topLeftCell="D15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8:W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -18399,7 +18399,7 @@
   </sheetPr>
   <dimension ref="A1:CK15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -20637,7 +20637,7 @@
   </sheetPr>
   <dimension ref="A1:CK30"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -24686,7 +24686,7 @@
   </sheetPr>
   <dimension ref="A1:CK9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
@@ -25888,8 +25888,8 @@
   </sheetPr>
   <dimension ref="A1:CI7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -25901,7 +25901,7 @@
     <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" s="77" customFormat="1" ht="53.25">
+    <row r="1" spans="1:87" s="77" customFormat="1" ht="55.15">
       <c r="A1" s="64" t="s">
         <v>529</v>
       </c>
@@ -25936,7 +25936,7 @@
         <v>532</v>
       </c>
       <c r="L1" s="69" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="M1" s="27" t="s">
         <v>533</v>
@@ -26582,7 +26582,7 @@
   </sheetPr>
   <dimension ref="A1:AS11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -27381,7 +27381,7 @@
   </sheetPr>
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="S2" sqref="S2:S7"/>
     </sheetView>
   </sheetViews>
@@ -28032,7 +28032,7 @@
   </sheetPr>
   <dimension ref="A1:CK44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="H26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -34268,16 +34268,12 @@
   </sheetData>
   <autoFilter ref="A1:CK1" xr:uid="{81481555-CC8D-496A-8B62-D9F1569CF07D}"/>
   <mergeCells count="28">
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q11:R11"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="Q16:R16"/>
@@ -34290,12 +34286,16 @@
     <mergeCell ref="Q24:R24"/>
     <mergeCell ref="Q25:R25"/>
     <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="Q33:R33"/>
   </mergeCells>
   <conditionalFormatting sqref="P1:R1">
     <cfRule type="expression" dxfId="28" priority="1" stopIfTrue="1">

</xml_diff>